<commit_message>
ng: update oncho stop forms.
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_oncho_bsc_202306_11_capture_niger.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2023/june/ng_oncho_bsc_202306_11_capture_niger.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bonhe\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\june\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2023\june\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279AA739-C7B3-4B46-A123-C5B17E3B6B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F86C549-465B-4F6C-8162-C2435740AE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="177">
   <si>
     <t>type</t>
   </si>
@@ -365,9 +365,6 @@
     <t>Collect the GPS</t>
   </si>
   <si>
-    <t>ng_oncho_bsc_202306_11_capture_niger</t>
-  </si>
-  <si>
     <t>NIGER</t>
   </si>
   <si>
@@ -521,10 +518,52 @@
     <t>NDASSA</t>
   </si>
   <si>
-    <t>CHOGI</t>
-  </si>
-  <si>
-    <t>(2023 July) - 11. (Niger) Human Landing Catches</t>
+    <t>ng_oncho_bsc_202306_11_capture_niger_v2</t>
+  </si>
+  <si>
+    <t>(2023 July) - 11. (Niger) Human Landing Catches V2</t>
+  </si>
+  <si>
+    <t>KOTANGORA</t>
+  </si>
+  <si>
+    <t>LAVUN</t>
+  </si>
+  <si>
+    <t>CHEGU</t>
+  </si>
+  <si>
+    <t>SINNA</t>
+  </si>
+  <si>
+    <t>YANGBA</t>
+  </si>
+  <si>
+    <t>BOSSO (PYATA)</t>
+  </si>
+  <si>
+    <t>MAITUMBI PRIMARY SCHOOL.</t>
+  </si>
+  <si>
+    <t>KOTANGORA IDP CAMP</t>
+  </si>
+  <si>
+    <t>SHESHI EWOWARA</t>
+  </si>
+  <si>
+    <t>TEGINA IDP CAMP</t>
+  </si>
+  <si>
+    <t>KEDE IDP CAMP</t>
+  </si>
+  <si>
+    <t>SHIRORO IDP CAMP</t>
+  </si>
+  <si>
+    <t>CHOGI (CHEJI)</t>
+  </si>
+  <si>
+    <t>D.LADIMA</t>
   </si>
 </sst>
 </file>
@@ -1522,11 +1561,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F85" sqref="F85:F119"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1798,10 +1837,10 @@
         <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1809,13 +1848,13 @@
         <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1823,13 +1862,13 @@
         <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1837,13 +1876,13 @@
         <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1851,13 +1890,13 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1865,13 +1904,13 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1879,13 +1918,13 @@
         <v>63</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1893,13 +1932,13 @@
         <v>63</v>
       </c>
       <c r="B34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1907,13 +1946,13 @@
         <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1921,13 +1960,13 @@
         <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1935,13 +1974,13 @@
         <v>63</v>
       </c>
       <c r="B37" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="C37" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1949,13 +1988,13 @@
         <v>63</v>
       </c>
       <c r="B38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1963,13 +2002,13 @@
         <v>63</v>
       </c>
       <c r="B39" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1977,13 +2016,13 @@
         <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C40" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1991,13 +2030,13 @@
         <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2005,13 +2044,13 @@
         <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2019,13 +2058,13 @@
         <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2033,13 +2072,13 @@
         <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2047,13 +2086,13 @@
         <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2061,13 +2100,13 @@
         <v>63</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C46" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2075,41 +2114,41 @@
         <v>63</v>
       </c>
       <c r="B47" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C47" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D47" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+      <c r="D48" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C49" t="s">
-        <v>132</v>
-      </c>
-      <c r="E49" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" t="s">
-        <v>133</v>
-      </c>
-      <c r="C50" t="s">
-        <v>133</v>
-      </c>
-      <c r="E50" t="s">
-        <v>113</v>
+        <v>130</v>
+      </c>
+      <c r="D49" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2117,13 +2156,13 @@
         <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C51" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E51" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2131,13 +2170,13 @@
         <v>64</v>
       </c>
       <c r="B52" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E52" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -2145,13 +2184,13 @@
         <v>64</v>
       </c>
       <c r="B53" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="C53" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -2159,13 +2198,13 @@
         <v>64</v>
       </c>
       <c r="B54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -2173,13 +2212,13 @@
         <v>64</v>
       </c>
       <c r="B55" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="C55" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="E55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2187,13 +2226,13 @@
         <v>64</v>
       </c>
       <c r="B56" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="E56" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -2201,13 +2240,13 @@
         <v>64</v>
       </c>
       <c r="B57" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C57" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E57" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -2215,13 +2254,13 @@
         <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -2229,13 +2268,13 @@
         <v>64</v>
       </c>
       <c r="B59" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="C59" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="E59" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -2243,13 +2282,13 @@
         <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="C60" t="s">
-        <v>117</v>
+        <v>138</v>
       </c>
       <c r="E60" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2257,13 +2296,13 @@
         <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C61" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E61" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2271,13 +2310,13 @@
         <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="C62" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="E62" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2285,13 +2324,13 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="C63" t="s">
-        <v>143</v>
+        <v>167</v>
       </c>
       <c r="E63" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -2299,13 +2338,13 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="C64" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E64" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2313,13 +2352,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="C65" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="E65" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2327,13 +2366,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="C66" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="E66" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2341,13 +2380,13 @@
         <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C67" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E67" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2355,13 +2394,13 @@
         <v>64</v>
       </c>
       <c r="B68" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C68" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2369,13 +2408,13 @@
         <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="C69" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E69" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2383,13 +2422,13 @@
         <v>64</v>
       </c>
       <c r="B70" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C70" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E70" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2397,13 +2436,13 @@
         <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="C71" t="s">
-        <v>125</v>
+        <v>170</v>
       </c>
       <c r="E71" t="s">
-        <v>125</v>
+        <v>163</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2411,13 +2450,13 @@
         <v>64</v>
       </c>
       <c r="B72" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C72" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E72" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2425,13 +2464,13 @@
         <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C73" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="E73" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2439,13 +2478,13 @@
         <v>64</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="E74" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2453,13 +2492,13 @@
         <v>64</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C75" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E75" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2467,13 +2506,13 @@
         <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E76" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2481,13 +2520,13 @@
         <v>64</v>
       </c>
       <c r="B77" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C77" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E77" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2495,13 +2534,13 @@
         <v>64</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="C78" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="E78" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2509,13 +2548,13 @@
         <v>64</v>
       </c>
       <c r="B79" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C79" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E79" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2523,13 +2562,13 @@
         <v>64</v>
       </c>
       <c r="B80" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="C80" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="E80" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2537,13 +2576,13 @@
         <v>64</v>
       </c>
       <c r="B81" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C81" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E81" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2551,13 +2590,13 @@
         <v>64</v>
       </c>
       <c r="B82" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C82" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E82" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2565,167 +2604,167 @@
         <v>64</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="C83" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="E83" t="s">
-        <v>131</v>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" t="s">
+        <v>64</v>
+      </c>
+      <c r="B84" t="s">
+        <v>152</v>
+      </c>
+      <c r="C84" t="s">
+        <v>152</v>
+      </c>
+      <c r="E84" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B85">
-        <v>301</v>
-      </c>
-      <c r="C85">
-        <v>301</v>
-      </c>
-      <c r="F85" t="s">
-        <v>132</v>
+      <c r="A85" t="s">
+        <v>64</v>
+      </c>
+      <c r="B85" t="s">
+        <v>153</v>
+      </c>
+      <c r="C85" t="s">
+        <v>153</v>
+      </c>
+      <c r="E85" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="1:6">
-      <c r="A86" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B86">
-        <v>302</v>
-      </c>
-      <c r="C86">
-        <v>302</v>
-      </c>
-      <c r="F86" t="s">
-        <v>133</v>
+      <c r="A86" t="s">
+        <v>64</v>
+      </c>
+      <c r="B86" t="s">
+        <v>176</v>
+      </c>
+      <c r="C86" t="s">
+        <v>154</v>
+      </c>
+      <c r="E86" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="87" spans="1:6">
-      <c r="A87" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B87">
-        <v>303</v>
-      </c>
-      <c r="C87">
-        <v>303</v>
-      </c>
-      <c r="F87" t="s">
-        <v>134</v>
+      <c r="A87" t="s">
+        <v>64</v>
+      </c>
+      <c r="B87" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" t="s">
+        <v>155</v>
+      </c>
+      <c r="E87" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="88" spans="1:6">
-      <c r="A88" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B88">
-        <v>304</v>
-      </c>
-      <c r="C88">
-        <v>304</v>
-      </c>
-      <c r="F88" t="s">
-        <v>135</v>
+      <c r="A88" t="s">
+        <v>64</v>
+      </c>
+      <c r="B88" t="s">
+        <v>156</v>
+      </c>
+      <c r="C88" t="s">
+        <v>156</v>
+      </c>
+      <c r="E88" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="89" spans="1:6">
-      <c r="A89" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B89">
-        <v>305</v>
-      </c>
-      <c r="C89">
-        <v>305</v>
-      </c>
-      <c r="F89" t="s">
-        <v>136</v>
+      <c r="A89" t="s">
+        <v>64</v>
+      </c>
+      <c r="B89" t="s">
+        <v>157</v>
+      </c>
+      <c r="C89" t="s">
+        <v>157</v>
+      </c>
+      <c r="E89" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B90">
-        <v>306</v>
-      </c>
-      <c r="C90">
-        <v>306</v>
-      </c>
-      <c r="F90" t="s">
-        <v>138</v>
+      <c r="A90" t="s">
+        <v>64</v>
+      </c>
+      <c r="B90" t="s">
+        <v>158</v>
+      </c>
+      <c r="C90" t="s">
+        <v>158</v>
+      </c>
+      <c r="E90" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="91" spans="1:6">
-      <c r="A91" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B91">
-        <v>307</v>
-      </c>
-      <c r="C91">
-        <v>307</v>
-      </c>
-      <c r="F91" t="s">
-        <v>140</v>
+      <c r="A91" t="s">
+        <v>64</v>
+      </c>
+      <c r="B91" t="s">
+        <v>159</v>
+      </c>
+      <c r="C91" t="s">
+        <v>159</v>
+      </c>
+      <c r="E91" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:6">
-      <c r="A92" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B92">
-        <v>308</v>
-      </c>
-      <c r="C92">
-        <v>308</v>
-      </c>
-      <c r="F92" t="s">
-        <v>141</v>
+      <c r="A92" t="s">
+        <v>64</v>
+      </c>
+      <c r="B92" t="s">
+        <v>160</v>
+      </c>
+      <c r="C92" t="s">
+        <v>160</v>
+      </c>
+      <c r="E92" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B93">
-        <v>309</v>
-      </c>
-      <c r="C93">
-        <v>309</v>
-      </c>
-      <c r="F93" t="s">
-        <v>143</v>
+      <c r="A93" t="s">
+        <v>64</v>
+      </c>
+      <c r="B93" t="s">
+        <v>174</v>
+      </c>
+      <c r="C93" t="s">
+        <v>174</v>
+      </c>
+      <c r="E93" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="94" spans="1:6">
-      <c r="A94" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B94">
-        <v>310</v>
-      </c>
-      <c r="C94">
-        <v>310</v>
-      </c>
-      <c r="F94" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B95">
-        <v>311</v>
-      </c>
-      <c r="C95">
-        <v>311</v>
-      </c>
-      <c r="F95" t="s">
-        <v>145</v>
+      <c r="A94" t="s">
+        <v>64</v>
+      </c>
+      <c r="B94" t="s">
+        <v>175</v>
+      </c>
+      <c r="C94" t="s">
+        <v>175</v>
+      </c>
+      <c r="E94" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2733,13 +2772,13 @@
         <v>100</v>
       </c>
       <c r="B96">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="C96">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="F96" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2747,13 +2786,13 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="C97">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="F97" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2761,13 +2800,13 @@
         <v>100</v>
       </c>
       <c r="B98">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="C98">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="F98" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2775,13 +2814,13 @@
         <v>100</v>
       </c>
       <c r="B99">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C99">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="F99" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2789,13 +2828,13 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="C100">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="F100" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2803,13 +2842,13 @@
         <v>100</v>
       </c>
       <c r="B101">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="C101">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="F101" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2817,13 +2856,13 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="C102">
-        <v>318</v>
+        <v>334</v>
       </c>
       <c r="F102" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2831,13 +2870,13 @@
         <v>100</v>
       </c>
       <c r="B103">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="C103">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="F103" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2845,13 +2884,13 @@
         <v>100</v>
       </c>
       <c r="B104">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="C104">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="F104" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2859,13 +2898,13 @@
         <v>100</v>
       </c>
       <c r="B105">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="C105">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="F105" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2873,13 +2912,13 @@
         <v>100</v>
       </c>
       <c r="B106">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="C106">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="F106" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2887,13 +2926,13 @@
         <v>100</v>
       </c>
       <c r="B107">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="C107">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="F107" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2901,13 +2940,13 @@
         <v>100</v>
       </c>
       <c r="B108">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="C108">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="F108" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2915,13 +2954,13 @@
         <v>100</v>
       </c>
       <c r="B109">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="C109">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="F109" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2929,13 +2968,13 @@
         <v>100</v>
       </c>
       <c r="B110">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="C110">
-        <v>326</v>
+        <v>309</v>
       </c>
       <c r="F110" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2943,13 +2982,13 @@
         <v>100</v>
       </c>
       <c r="B111">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="C111">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="F111" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2957,13 +2996,13 @@
         <v>100</v>
       </c>
       <c r="B112">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="C112">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="F112" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2971,13 +3010,13 @@
         <v>100</v>
       </c>
       <c r="B113">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="C113">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="F113" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2985,13 +3024,13 @@
         <v>100</v>
       </c>
       <c r="B114">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="C114">
-        <v>330</v>
+        <v>313</v>
       </c>
       <c r="F114" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2999,13 +3038,13 @@
         <v>100</v>
       </c>
       <c r="B115">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="C115">
-        <v>331</v>
+        <v>314</v>
       </c>
       <c r="F115" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3013,13 +3052,13 @@
         <v>100</v>
       </c>
       <c r="B116">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="C116">
-        <v>332</v>
+        <v>315</v>
       </c>
       <c r="F116" t="s">
-        <v>117</v>
+        <v>148</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3027,13 +3066,13 @@
         <v>100</v>
       </c>
       <c r="B117">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="C117">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="F117" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3041,13 +3080,13 @@
         <v>100</v>
       </c>
       <c r="B118">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C118">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F118" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3055,24 +3094,298 @@
         <v>100</v>
       </c>
       <c r="B119">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="C119">
-        <v>335</v>
+        <v>317</v>
       </c>
       <c r="F119" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="120" spans="1:6">
-      <c r="A120" s="13"/>
+      <c r="A120" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B120">
+        <v>318</v>
+      </c>
+      <c r="C120">
+        <v>318</v>
+      </c>
+      <c r="F120" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="121" spans="1:6">
-      <c r="A121" s="13"/>
+      <c r="A121" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B121">
+        <v>319</v>
+      </c>
+      <c r="C121">
+        <v>319</v>
+      </c>
+      <c r="F121" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B122">
+        <v>320</v>
+      </c>
+      <c r="C122">
+        <v>320</v>
+      </c>
+      <c r="F122" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B123">
+        <v>321</v>
+      </c>
+      <c r="C123">
+        <v>321</v>
+      </c>
+      <c r="F123" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B124">
+        <v>329</v>
+      </c>
+      <c r="C124">
+        <v>329</v>
+      </c>
+      <c r="F124" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B125">
+        <v>322</v>
+      </c>
+      <c r="C125">
+        <v>322</v>
+      </c>
+      <c r="F125" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B126">
+        <v>323</v>
+      </c>
+      <c r="C126">
+        <v>323</v>
+      </c>
+      <c r="F126" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B127">
+        <v>324</v>
+      </c>
+      <c r="C127">
+        <v>324</v>
+      </c>
+      <c r="F127" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B128">
+        <v>325</v>
+      </c>
+      <c r="C128">
+        <v>325</v>
+      </c>
+      <c r="F128" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B129">
+        <v>326</v>
+      </c>
+      <c r="C129">
+        <v>326</v>
+      </c>
+      <c r="F129" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B130">
+        <v>327</v>
+      </c>
+      <c r="C130">
+        <v>327</v>
+      </c>
+      <c r="F130" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B131">
+        <v>350</v>
+      </c>
+      <c r="C131">
+        <v>350</v>
+      </c>
+      <c r="F131" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B132">
+        <v>351</v>
+      </c>
+      <c r="C132">
+        <v>351</v>
+      </c>
+      <c r="F132" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B133">
+        <v>352</v>
+      </c>
+      <c r="C133">
+        <v>352</v>
+      </c>
+      <c r="F133" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B134">
+        <v>353</v>
+      </c>
+      <c r="C134">
+        <v>353</v>
+      </c>
+      <c r="F134" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B135">
+        <v>354</v>
+      </c>
+      <c r="C135">
+        <v>354</v>
+      </c>
+      <c r="F135" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B136">
+        <v>355</v>
+      </c>
+      <c r="C136">
+        <v>355</v>
+      </c>
+      <c r="F136" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B137">
+        <v>356</v>
+      </c>
+      <c r="C137">
+        <v>356</v>
+      </c>
+      <c r="F137" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B138">
+        <v>357</v>
+      </c>
+      <c r="C138">
+        <v>357</v>
+      </c>
+      <c r="F138" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B139">
+        <v>358</v>
+      </c>
+      <c r="C139">
+        <v>358</v>
+      </c>
+      <c r="F139" t="s">
+        <v>169</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A61:B97">
-    <sortCondition ref="B61:B97"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A63:B108">
+    <sortCondition ref="B63:B108"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3083,14 +3396,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="44.125" customWidth="1"/>
-    <col min="2" max="2" width="34.75" customWidth="1"/>
+    <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3106,10 +3419,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>86</v>

</xml_diff>